<commit_message>
updated the type for 2 repos
</commit_message>
<xml_diff>
--- a/manual_classification/Manual_Classification_tbs.xlsx
+++ b/manual_classification/Manual_Classification_tbs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maria/Documents/dottorato/progetto_complementiIS_2020/consegna/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E830C6-E733-D646-85E9-CC1BC29B8097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76FE31E-9ABC-5047-973E-7D51D1662DD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Foglio 1 - Manual_Classificatio'!$D$1:$D$1509</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -18374,8 +18366,8 @@
   </sheetPr>
   <dimension ref="A1:F1509"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1422" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1439" sqref="A1439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23685,7 +23677,7 @@
         <v>6</v>
       </c>
       <c r="F265" s="9" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
     </row>
     <row r="266" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -47165,7 +47157,7 @@
         <v>4</v>
       </c>
       <c r="F1439" s="18" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1440" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>